<commit_message>
add JDD, fix supermarket
</commit_message>
<xml_diff>
--- a/supermarket/prj/code/tune log.xlsx
+++ b/supermarket/prj/code/tune log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
   <si>
     <t>序号</t>
   </si>
@@ -46,6 +46,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">4.4：0.1547
 4.5：0.2156
 4.6: 0.2592
@@ -109,6 +116,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>4.4：0.1419
 4.5：0.2126
 4.6: 0.2621</t>
@@ -169,6 +183,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>4.4：0.1062
 4.5：0.1479
 4.6: 0.2480</t>
@@ -207,6 +228,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>4.4：0.1021
 4.5：0.1284
 4.6: 0.2206</t>
@@ -234,18 +262,83 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>单独预测coupon相关类，用coupon特征，
+异常值过滤修正：（-2,3），14天平滑</t>
+  </si>
+  <si>
+    <t>单独预测coupon相关类，用coupon特征，
+异常值过滤修正：（-2,3），
+7天平滑</t>
+  </si>
+  <si>
+    <t>单独预测coupon相关类，用coupon特征，
+异常值过滤修正:（-1.5,1.5）
+14天平滑</t>
+  </si>
+  <si>
+    <t>单独预测coupon相关类，用coupon特征，
+异常值过滤修正：（-2,2）
+14天平滑</t>
+  </si>
+  <si>
+    <t>单独预测coupon相关类，用coupon特征，
+异常值过滤修正：（-3,3）
+14天平滑</t>
+  </si>
+  <si>
+    <t>单独预测coupon相关类，用coupon特征，
+异常值过滤修正：（-2,2）
+14天平滑，排除过年17,18号</t>
+  </si>
+  <si>
+    <t>单独预测coupon相关类，用coupon特征，
+异常值过滤修正：（-2,2）
+7天平滑</t>
+  </si>
+  <si>
+    <t>单独预测coupon相关类，排除coupon特征，
+异常值过滤修正：（-2,2）
+14天平滑</t>
+  </si>
+  <si>
+    <t>全部预测，用coupon特征，
+异常值过滤修正:（-1.5,1.5）
+14天平滑</t>
+  </si>
+  <si>
+    <t>全部预测，用coupon特征，
+异常值过滤修正:（-2,2）
+14天平滑</t>
+  </si>
+  <si>
+    <t>Coupon特征比较糟糕</t>
+  </si>
+  <si>
+    <t>单独预测非coupon相关类
+异常值过滤修正：（-2,2）
+14天平滑</t>
+  </si>
+  <si>
+    <t>coupon,非coupon分两拨预测，
+(-1.5,1.5),(-2,2),14天平滑</t>
+  </si>
+  <si>
+    <t>coupon特征对于有促销的商品有积极作用，
+对于非促销起消极作用</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,9 +355,144 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,161 +508,33 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="2" tint="-0.5"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <color theme="5" tint="0.4"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="2" tint="-0.5"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="5" tint="0.4"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,187 +543,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,17 +758,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -697,11 +797,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -736,7 +842,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -757,10 +863,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -769,137 +875,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -907,12 +1013,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -926,6 +1026,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1275,13 +1387,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:F7"/>
+  <dimension ref="A2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
     <col min="2" max="2" width="27.125" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
@@ -1296,12 +1408,12 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1"/>
@@ -1315,81 +1427,183 @@
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" ht="117" customHeight="1" spans="1:6">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>0.1725</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>0.18627980456</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" ht="94.5" spans="1:6">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
         <v>0.190493312411</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" ht="67.5" spans="1:6">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
         <v>0.14082899947</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" ht="67.5" spans="1:6">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
         <v>0.13074962623</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" ht="54" spans="2:4">
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>0.1728</v>
+      </c>
+    </row>
+    <row r="9" ht="54" spans="2:2">
+      <c r="B9" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" ht="54" spans="2:4">
+      <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.176</v>
+      </c>
+    </row>
+    <row r="11" ht="54" spans="2:4">
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>0.176</v>
+      </c>
+    </row>
+    <row r="12" ht="54" spans="2:4">
+      <c r="B12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>0.1708</v>
+      </c>
+    </row>
+    <row r="13" ht="54" spans="2:4">
+      <c r="B13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>0.1737</v>
+      </c>
+    </row>
+    <row r="14" ht="54" spans="2:4">
+      <c r="B14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>0.1754</v>
+      </c>
+    </row>
+    <row r="15" ht="54" spans="2:4">
+      <c r="B15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15">
+        <v>0.16995</v>
+      </c>
+    </row>
+    <row r="16" ht="40.5" spans="2:4">
+      <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16">
+        <v>0.18007</v>
+      </c>
+    </row>
+    <row r="17" ht="40.5" spans="2:6">
+      <c r="B17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17">
+        <v>0.169</v>
+      </c>
+      <c r="D17">
+        <v>0.1803</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" ht="40.5" spans="2:4">
+      <c r="B18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18">
+        <v>0.1887</v>
+      </c>
+    </row>
+    <row r="19" ht="27" spans="2:6">
+      <c r="B19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <v>0.18172</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>